<commit_message>
Ajuste do processo para executar apenas em uma unica chamada2
</commit_message>
<xml_diff>
--- a/Banco/IPs_PDVs.xlsx
+++ b/Banco/IPs_PDVs.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -461,32 +461,32 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
+          <t>StatusEnvio</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
           <t>Conexão</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>StatusEnvio</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>5246</v>
+        <v>5265</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>L5246 - SWIFT GERMINARE</t>
+          <t>L5265 - SWIFT FLAMBOYANT (GO)</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>PDV 05</t>
+          <t>PDV 01</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>10.253.16.50</t>
+          <t>10.240.147.83</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -494,10 +494,80 @@
           <t>Ping OK</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr"/>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Enviado</t>
+        </is>
+      </c>
       <c r="G2" t="inlineStr">
         <is>
+          <t>Conectado</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>5244</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>L5244 - SWIFT TAGUATINGA SUL (DF)</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>PDV 03</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>10.240.134.31</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Ping OK</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
           <t>Enviado</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Conectado</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>5259</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>L5259 - SWIFT ALL WAYS MALL (RJ)</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>PDV 02</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>10.240.132.156</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Enviado</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Conectado</t>
         </is>
       </c>
     </row>

</xml_diff>